<commit_message>
rilettura di tutit i diari, continuazione con la doc, modifiche commeni ai codici
</commit_message>
<xml_diff>
--- a/Progettazione/Analisi/test.xlsx
+++ b/Progettazione/Analisi/test.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="23">
   <si>
     <t>TC-001</t>
   </si>
@@ -67,26 +67,29 @@
     <t>TC-017</t>
   </si>
   <si>
-    <t>test</t>
-  </si>
-  <si>
-    <t>risultato</t>
-  </si>
-  <si>
-    <t>osservazioni</t>
-  </si>
-  <si>
-    <t>ok</t>
-  </si>
-  <si>
-    <t>ottimizzato su Chrome</t>
+    <t>Passato</t>
+  </si>
+  <si>
+    <t>Test</t>
+  </si>
+  <si>
+    <t>Risultato</t>
+  </si>
+  <si>
+    <t>Osservazioni</t>
+  </si>
+  <si>
+    <t>Ottimizzato su Chrome</t>
+  </si>
+  <si>
+    <t>Segnalato più avanti</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -94,16 +97,29 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="14">
     <border>
       <left/>
       <right/>
@@ -111,12 +127,225 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normale" xfId="0" builtinId="0"/>
@@ -421,153 +650,226 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:D18"/>
+  <dimension ref="B1:G18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+      <selection activeCell="B1" sqref="B1:E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="5" max="5" width="11.77734375" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B1" t="s">
-        <v>17</v>
-      </c>
-      <c r="C1" t="s">
+    <row r="1" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B1" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="D1" t="s">
+      <c r="C1" s="5" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="2" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B2" t="s">
+      <c r="D1" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="E1" s="11"/>
+      <c r="G1" s="14"/>
+    </row>
+    <row r="2" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B2" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="C2" t="s">
-        <v>20</v>
-      </c>
-      <c r="D2" t="s">
+      <c r="C2" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D2" s="12" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="3" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B3" t="s">
+      <c r="E2" s="13"/>
+    </row>
+    <row r="3" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B3" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="C3" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="4" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B4" t="s">
+      <c r="C3" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D3" s="12"/>
+      <c r="E3" s="13"/>
+    </row>
+    <row r="4" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B4" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="C4" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="5" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B5" t="s">
+      <c r="C4" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D4" s="12"/>
+      <c r="E4" s="13"/>
+    </row>
+    <row r="5" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B5" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="C5" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="6" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B6" t="s">
+      <c r="C5" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D5" s="12"/>
+      <c r="E5" s="13"/>
+    </row>
+    <row r="6" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B6" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="C6" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="7" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B7" t="s">
+      <c r="C6" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D6" s="12"/>
+      <c r="E6" s="13"/>
+    </row>
+    <row r="7" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B7" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="C7" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="8" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B8" t="s">
+      <c r="C7" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D7" s="12"/>
+      <c r="E7" s="13"/>
+    </row>
+    <row r="8" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B8" s="6" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="9" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B9" t="s">
+      <c r="C8" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D8" s="12"/>
+      <c r="E8" s="13"/>
+    </row>
+    <row r="9" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B9" s="6" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="10" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B10" t="s">
+      <c r="C9" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D9" s="12"/>
+      <c r="E9" s="13"/>
+    </row>
+    <row r="10" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B10" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="C10" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="11" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B11" t="s">
+      <c r="C10" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D10" s="12"/>
+      <c r="E10" s="13"/>
+    </row>
+    <row r="11" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B11" s="6" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="12" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B12" t="s">
+      <c r="C11" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D11" s="12"/>
+      <c r="E11" s="13"/>
+    </row>
+    <row r="12" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B12" s="6" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="13" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B13" t="s">
+      <c r="C12" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="E12" s="7"/>
+    </row>
+    <row r="13" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B13" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="C13" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="14" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B14" t="s">
+      <c r="C13" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="E13" s="7"/>
+    </row>
+    <row r="14" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B14" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="C14" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="15" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B15" t="s">
+      <c r="C14" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D14" s="12"/>
+      <c r="E14" s="13"/>
+    </row>
+    <row r="15" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B15" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="C15" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="16" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B16" t="s">
+      <c r="C15" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D15" s="12"/>
+      <c r="E15" s="13"/>
+    </row>
+    <row r="16" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B16" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="C16" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="17" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B17" t="s">
+      <c r="C16" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D16" s="12"/>
+      <c r="E16" s="13"/>
+    </row>
+    <row r="17" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B17" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="C17" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="18" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B18" t="s">
+      <c r="C17" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D17" s="12"/>
+      <c r="E17" s="13"/>
+    </row>
+    <row r="18" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B18" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="C18" t="s">
-        <v>20</v>
-      </c>
+      <c r="C18" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="D18" s="15"/>
+      <c r="E18" s="16"/>
     </row>
   </sheetData>
+  <mergeCells count="16">
+    <mergeCell ref="D10:E10"/>
+    <mergeCell ref="D9:E9"/>
+    <mergeCell ref="D18:E18"/>
+    <mergeCell ref="D17:E17"/>
+    <mergeCell ref="D16:E16"/>
+    <mergeCell ref="D15:E15"/>
+    <mergeCell ref="D14:E14"/>
+    <mergeCell ref="D11:E11"/>
+    <mergeCell ref="D1:E1"/>
+    <mergeCell ref="D2:E2"/>
+    <mergeCell ref="D8:E8"/>
+    <mergeCell ref="D7:E7"/>
+    <mergeCell ref="D6:E6"/>
+    <mergeCell ref="D5:E5"/>
+    <mergeCell ref="D4:E4"/>
+    <mergeCell ref="D3:E3"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>